<commit_message>
constructor invocation return type set to instance type
</commit_message>
<xml_diff>
--- a/selected_bytecodes.xlsx
+++ b/selected_bytecodes.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="dup" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="118">
   <si>
     <t>Mnemonic</t>
   </si>
@@ -2245,6 +2246,60 @@
   </si>
   <si>
     <t>extracted</t>
+  </si>
+  <si>
+    <t>dup</t>
+  </si>
+  <si>
+    <t>value → value, value</t>
+  </si>
+  <si>
+    <t>duplicate the value on top of the stack</t>
+  </si>
+  <si>
+    <t>dup_x1</t>
+  </si>
+  <si>
+    <t>value2, value1 → value1, value2, value1</t>
+  </si>
+  <si>
+    <t>insert a copy of the top value into the stack two values from the top. value1 and value2 must not be of the type double or long.</t>
+  </si>
+  <si>
+    <t>dup_x2</t>
+  </si>
+  <si>
+    <t>value3, value2, value1 → value1, value3, value2, value1</t>
+  </si>
+  <si>
+    <t>insert a copy of the top value into the stack two (if value2 is double or long it takes up the entry of value3, too) or three values (if value2 is neither double nor long) from the top</t>
+  </si>
+  <si>
+    <t>dup2</t>
+  </si>
+  <si>
+    <t>{value2, value1} → {value2, value1}, {value2, value1}</t>
+  </si>
+  <si>
+    <t>duplicate top two stack words (two values, if value1 is not double nor long; a single value, if value1 is double or long)</t>
+  </si>
+  <si>
+    <t>dup2_x1</t>
+  </si>
+  <si>
+    <t>value3, {value2, value1} → {value2, value1}, value3, {value2, value1}</t>
+  </si>
+  <si>
+    <t>duplicate two words and insert beneath third word (see explanation above)</t>
+  </si>
+  <si>
+    <t>dup2_x2</t>
+  </si>
+  <si>
+    <t>{value4, value3}, {value2, value1} → {value2, value1}, {value4, value3}, {value2, value1}</t>
+  </si>
+  <si>
+    <t>duplicate two words and insert beneath fourth word</t>
   </si>
 </sst>
 </file>
@@ -2388,13 +2443,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2678,7 +2733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A53" workbookViewId="0">
       <selection activeCell="I21" sqref="I21:I36"/>
     </sheetView>
   </sheetViews>
@@ -2694,24 +2749,24 @@
   <sheetData>
     <row r="3" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="5"/>
+      <c r="E4" s="6"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="6"/>
+      <c r="C5" s="7"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="6"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="6"/>
+      <c r="H5" s="7"/>
       <c r="I5" t="s">
         <v>99</v>
       </c>
@@ -2727,7 +2782,7 @@
       <c r="H6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="3:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="4" t="s">
@@ -2740,7 +2795,7 @@
       <c r="H7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="4" t="s">
@@ -2861,7 +2916,7 @@
       <c r="H17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="I17" s="5"/>
     </row>
     <row r="18" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="4" t="s">
@@ -2874,7 +2929,7 @@
       <c r="H18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I18" s="7"/>
+      <c r="I18" s="5"/>
     </row>
     <row r="19" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="4" t="s">
@@ -2887,7 +2942,7 @@
       <c r="H19" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I19" s="7"/>
+      <c r="I19" s="5"/>
     </row>
     <row r="20" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="4" t="s">
@@ -2900,7 +2955,7 @@
       <c r="H20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I20" s="7"/>
+      <c r="I20" s="5"/>
     </row>
     <row r="21" spans="3:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="4" t="s">
@@ -2913,7 +2968,7 @@
       <c r="H21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I21" s="7"/>
+      <c r="I21" s="5"/>
     </row>
     <row r="22" spans="3:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="4" t="s">
@@ -2926,7 +2981,7 @@
       <c r="H22" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I22" s="7"/>
+      <c r="I22" s="5"/>
     </row>
     <row r="23" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="4" t="s">
@@ -2939,7 +2994,7 @@
       <c r="H23" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I23" s="7"/>
+      <c r="I23" s="5"/>
     </row>
     <row r="24" spans="3:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="4" t="s">
@@ -2952,7 +3007,7 @@
       <c r="H24" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I24" s="7"/>
+      <c r="I24" s="5"/>
     </row>
     <row r="25" spans="3:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="4" t="s">
@@ -2965,7 +3020,7 @@
       <c r="H25" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I25" s="7"/>
+      <c r="I25" s="5"/>
     </row>
     <row r="26" spans="3:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="4" t="s">
@@ -2978,7 +3033,7 @@
       <c r="H26" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I26" s="7"/>
+      <c r="I26" s="5"/>
     </row>
     <row r="27" spans="3:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="4" t="s">
@@ -2991,7 +3046,7 @@
       <c r="H27" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I27" s="7"/>
+      <c r="I27" s="5"/>
     </row>
     <row r="28" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="4" t="s">
@@ -3004,7 +3059,7 @@
       <c r="H28" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="I28" s="7"/>
+      <c r="I28" s="5"/>
     </row>
     <row r="29" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="4" t="s">
@@ -3017,7 +3072,7 @@
       <c r="H29" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I29" s="7"/>
+      <c r="I29" s="5"/>
     </row>
     <row r="30" spans="3:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="4" t="s">
@@ -3030,7 +3085,7 @@
       <c r="H30" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I30" s="7"/>
+      <c r="I30" s="5"/>
     </row>
     <row r="31" spans="3:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="4" t="s">
@@ -3043,7 +3098,7 @@
       <c r="H31" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I31" s="7"/>
+      <c r="I31" s="5"/>
     </row>
     <row r="32" spans="3:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="4" t="s">
@@ -3056,7 +3111,7 @@
       <c r="H32" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="I32" s="7"/>
+      <c r="I32" s="5"/>
     </row>
     <row r="33" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="4" t="s">
@@ -3069,7 +3124,7 @@
       <c r="H33" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="I33" s="7"/>
+      <c r="I33" s="5"/>
     </row>
     <row r="34" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="4" t="s">
@@ -3082,7 +3137,7 @@
       <c r="H34" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I34" s="7"/>
+      <c r="I34" s="5"/>
     </row>
     <row r="35" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="4" t="s">
@@ -3095,7 +3150,7 @@
       <c r="H35" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I35" s="7"/>
+      <c r="I35" s="5"/>
     </row>
     <row r="36" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="4" t="s">
@@ -3108,7 +3163,7 @@
       <c r="H36" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="I36" s="7"/>
+      <c r="I36" s="5"/>
     </row>
     <row r="37" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="4" t="s">
@@ -3133,7 +3188,7 @@
       <c r="H38" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="I38" s="7"/>
+      <c r="I38" s="5"/>
     </row>
     <row r="39" spans="3:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="4" t="s">
@@ -3146,7 +3201,7 @@
       <c r="H39" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="I39" s="7"/>
+      <c r="I39" s="5"/>
     </row>
     <row r="40" spans="3:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="4" t="s">
@@ -3159,7 +3214,7 @@
       <c r="H40" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="I40" s="7"/>
+      <c r="I40" s="5"/>
     </row>
     <row r="41" spans="3:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="4" t="s">
@@ -3172,7 +3227,7 @@
       <c r="H41" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="I41" s="7"/>
+      <c r="I41" s="5"/>
     </row>
     <row r="42" spans="3:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="4" t="s">
@@ -3185,7 +3240,7 @@
       <c r="H42" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="I42" s="7"/>
+      <c r="I42" s="5"/>
     </row>
     <row r="43" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="4" t="s">
@@ -3340,4 +3395,91 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="65.7109375" customWidth="1"/>
+    <col min="5" max="5" width="109.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added most of the instructions
</commit_message>
<xml_diff>
--- a/selected_bytecodes.xlsx
+++ b/selected_bytecodes.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="dup" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="208">
   <si>
     <t>Mnemonic</t>
   </si>
@@ -2300,13 +2301,503 @@
   </si>
   <si>
     <t>duplicate two words and insert beneath fourth word</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>aaload</t>
+  </si>
+  <si>
+    <t>stack pops</t>
+  </si>
+  <si>
+    <t>stack pushes</t>
+  </si>
+  <si>
+    <t>push type</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>aastore</t>
+  </si>
+  <si>
+    <t>aconst_null</t>
+  </si>
+  <si>
+    <t>descriptiion</t>
+  </si>
+  <si>
+    <r>
+      <t>Load </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>reference</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> from array</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Store into </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>reference</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> array</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Push </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>null</t>
+    </r>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>aload</t>
+  </si>
+  <si>
+    <r>
+      <t>Load </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>reference</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> from local variable</t>
+    </r>
+  </si>
+  <si>
+    <t>aload_&lt;n&gt;</t>
+  </si>
+  <si>
+    <t>anewarray</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>aload index</t>
+  </si>
+  <si>
+    <t>Create new array of reference</t>
+  </si>
+  <si>
+    <t>areturn</t>
+  </si>
+  <si>
+    <t>arraylength</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Get length of array</t>
+  </si>
+  <si>
+    <t>astore</t>
+  </si>
+  <si>
+    <t>astore_&lt;n&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t>Store </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>reference</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> into local variable</t>
+    </r>
+  </si>
+  <si>
+    <t>Throw exception or error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">similar instructions </t>
+  </si>
+  <si>
+    <t>bipush</t>
+  </si>
+  <si>
+    <t>Push byte</t>
+  </si>
+  <si>
+    <t>b,c,d,f,I,l,s</t>
+  </si>
+  <si>
+    <t>i.l</t>
+  </si>
+  <si>
+    <t>double to float</t>
+  </si>
+  <si>
+    <t>f,I,l</t>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/javase/specs/jvms/se7/html/jvms-6.html#jvms-6.5.goto</t>
+  </si>
+  <si>
+    <t>dcmp&lt;op&gt;</t>
+  </si>
+  <si>
+    <t>dcmpg/dcmpgl</t>
+  </si>
+  <si>
+    <t>dconst_&lt;d&gt;</t>
+  </si>
+  <si>
+    <t>push double</t>
+  </si>
+  <si>
+    <t>Duplicate the top operand stack value</t>
+  </si>
+  <si>
+    <t>special</t>
+  </si>
+  <si>
+    <t>Duplicate the top operand stack value and insert two values down v2,v1 -&gt; v1,v2,v1</t>
+  </si>
+  <si>
+    <t>Duplicate the top operand stack value and insert two or three values down depending on the length of the type.  For our purposes it will always be 2 values</t>
+  </si>
+  <si>
+    <t>Duplicate the top 2 operand stack values</t>
+  </si>
+  <si>
+    <t>Duplicate the top 2 operand stack values and insert two values down v2,v1 -&gt; v1,v2,v1</t>
+  </si>
+  <si>
+    <t>Duplicate the top 2 operand stack values and insert two or three values down depending on the length of the type.  For our purposes it will always be 2 values</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <r>
+      <t>Get </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>static</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> field from class</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Get </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>field from class</t>
+    </r>
+  </si>
+  <si>
+    <t>goto, goto_w</t>
+  </si>
+  <si>
+    <t>Branch always</t>
+  </si>
+  <si>
+    <t>f,I,l,</t>
+  </si>
+  <si>
+    <t>d2f, f2d, 12b, …</t>
+  </si>
+  <si>
+    <t>if_acmp&lt;cond&gt;</t>
+  </si>
+  <si>
+    <t>if_icmp&lt;cond&gt;</t>
+  </si>
+  <si>
+    <t>if&lt;cond&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t>Branch if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>reference</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>null</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Branch if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>reference</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> is not </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>null</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Branch if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> comparison with zero succeeds</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Branch if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> comparison succeeds</t>
+    </r>
+  </si>
+  <si>
+    <t>iinc</t>
+  </si>
+  <si>
+    <t>Increment local variable by constant</t>
+  </si>
+  <si>
+    <t>Invoke dynamic method  - not used</t>
+  </si>
+  <si>
+    <t>1+param count</t>
+  </si>
+  <si>
+    <t>param count</t>
+  </si>
+  <si>
+    <t>ior</t>
+  </si>
+  <si>
+    <t>Boolean OR int</t>
+  </si>
+  <si>
+    <t>Return reference from method and push onto the operand stack of the frame of the invoker</t>
+  </si>
+  <si>
+    <t>jsr, jsr_w</t>
+  </si>
+  <si>
+    <t>ishl, ishr, iushr, ixor, land, iand …</t>
+  </si>
+  <si>
+    <t>logical operations</t>
+  </si>
+  <si>
+    <t>Push item from run-time constant pool</t>
+  </si>
+  <si>
+    <t>ldc, ldc_w, ldc2_w</t>
+  </si>
+  <si>
+    <t>lookupswitch</t>
+  </si>
+  <si>
+    <t># of element counts</t>
+  </si>
+  <si>
+    <t>nop</t>
+  </si>
+  <si>
+    <t>pop, pop2</t>
+  </si>
+  <si>
+    <t>Set field in object</t>
+  </si>
+  <si>
+    <t>Set static field in class</t>
+  </si>
+  <si>
+    <t>sipush</t>
+  </si>
+  <si>
+    <t>push short</t>
+  </si>
+  <si>
+    <t>swap</t>
+  </si>
+  <si>
+    <t>Swap the top two operand stack values</t>
+  </si>
+  <si>
+    <t>wide</t>
+  </si>
+  <si>
+    <t>Extend local variable index by additional bytes</t>
+  </si>
+  <si>
+    <t>jump subroutine - in finally - not used in newer java versions 6+</t>
+  </si>
+  <si>
+    <t>Return from subroutine - see jsr</t>
+  </si>
+  <si>
+    <t>Access jump table by key match and jump - ignored for the moment</t>
+  </si>
+  <si>
+    <t>Access jump table by index and jump - ignored for the moment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2348,8 +2839,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2371,6 +2881,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2429,7 +2945,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2444,12 +2960,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2749,24 +3271,24 @@
   <sheetData>
     <row r="3" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="6"/>
+      <c r="E4" s="9"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="7"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="10"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="7"/>
+      <c r="H5" s="10"/>
       <c r="I5" t="s">
         <v>99</v>
       </c>
@@ -3401,7 +3923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -3482,4 +4004,874 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:J66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F45" workbookViewId="0">
+      <selection activeCell="J65" sqref="J65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" customWidth="1"/>
+    <col min="9" max="9" width="33.28515625" customWidth="1"/>
+    <col min="10" max="10" width="108.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" t="s">
+        <v>121</v>
+      </c>
+      <c r="H3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="5"/>
+      <c r="D5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" t="s">
+        <v>149</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="5"/>
+      <c r="D6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>149</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="5"/>
+      <c r="D7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>130</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="5"/>
+      <c r="D8" t="s">
+        <v>131</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>123</v>
+      </c>
+      <c r="I8" t="s">
+        <v>149</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="5"/>
+      <c r="D9" t="s">
+        <v>133</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>123</v>
+      </c>
+      <c r="I9" t="s">
+        <v>149</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="5"/>
+      <c r="D10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>123</v>
+      </c>
+      <c r="J10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="5"/>
+      <c r="D11" t="s">
+        <v>138</v>
+      </c>
+      <c r="I11" t="s">
+        <v>149</v>
+      </c>
+      <c r="J11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="5"/>
+      <c r="D12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>140</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="5"/>
+      <c r="D13" t="s">
+        <v>142</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>149</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="5"/>
+      <c r="D14" t="s">
+        <v>143</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
+        <v>149</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="5"/>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="5"/>
+      <c r="D16" t="s">
+        <v>147</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="5"/>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="5"/>
+      <c r="D18" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>150</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="5"/>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>123</v>
+      </c>
+      <c r="I19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C20" s="5"/>
+      <c r="D20" t="s">
+        <v>154</v>
+      </c>
+      <c r="E20" t="s">
+        <v>155</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="I20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C21" s="5"/>
+      <c r="D21" t="s">
+        <v>156</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>152</v>
+      </c>
+      <c r="J21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="5"/>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C23" s="5"/>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="5"/>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C25" s="5"/>
+      <c r="D25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C26" s="5"/>
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="I26" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C27" s="5"/>
+      <c r="D27" t="s">
+        <v>100</v>
+      </c>
+      <c r="F27" t="s">
+        <v>159</v>
+      </c>
+      <c r="G27" t="s">
+        <v>159</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C28" s="5"/>
+      <c r="D28" t="s">
+        <v>103</v>
+      </c>
+      <c r="F28" t="s">
+        <v>159</v>
+      </c>
+      <c r="G28" t="s">
+        <v>159</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C29" s="5"/>
+      <c r="D29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29" t="s">
+        <v>159</v>
+      </c>
+      <c r="G29" t="s">
+        <v>159</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C30" s="5"/>
+      <c r="D30" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" t="s">
+        <v>159</v>
+      </c>
+      <c r="G30" t="s">
+        <v>159</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C31" s="5"/>
+      <c r="D31" t="s">
+        <v>112</v>
+      </c>
+      <c r="F31" t="s">
+        <v>159</v>
+      </c>
+      <c r="G31" t="s">
+        <v>159</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C32" s="5"/>
+      <c r="D32" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" t="s">
+        <v>159</v>
+      </c>
+      <c r="G32" t="s">
+        <v>159</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C33" s="5"/>
+      <c r="D33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>165</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="5"/>
+      <c r="D34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>165</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C35" s="5"/>
+      <c r="D35" t="s">
+        <v>168</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C36" s="5"/>
+      <c r="D36" t="s">
+        <v>172</v>
+      </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C37" s="5"/>
+      <c r="D37" t="s">
+        <v>173</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C38" s="5"/>
+      <c r="D38" t="s">
+        <v>174</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C39" s="5"/>
+      <c r="D39" t="s">
+        <v>59</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C40" s="5"/>
+      <c r="D40" t="s">
+        <v>61</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C41" s="5"/>
+      <c r="D41" t="s">
+        <v>179</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C42" s="5"/>
+      <c r="D42" t="s">
+        <v>63</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>65</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C44" s="5"/>
+      <c r="D44" t="s">
+        <v>67</v>
+      </c>
+      <c r="F44" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C45" s="5"/>
+      <c r="D45" t="s">
+        <v>69</v>
+      </c>
+      <c r="F45" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C46" s="5"/>
+      <c r="D46" t="s">
+        <v>71</v>
+      </c>
+      <c r="F46" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C47" s="5"/>
+      <c r="D47" t="s">
+        <v>73</v>
+      </c>
+      <c r="F47" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C48" s="5"/>
+      <c r="D48" t="s">
+        <v>184</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="J48" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C49" s="5"/>
+      <c r="D49" t="s">
+        <v>188</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C50" s="11"/>
+      <c r="D50" t="s">
+        <v>187</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="J50" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C51" s="5"/>
+      <c r="D51" t="s">
+        <v>191</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>192</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C53" s="5"/>
+      <c r="D53" t="s">
+        <v>79</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C54" s="5"/>
+      <c r="D54" t="s">
+        <v>81</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C55" s="5"/>
+      <c r="D55" t="s">
+        <v>83</v>
+      </c>
+      <c r="F55" t="s">
+        <v>193</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C56" s="5"/>
+      <c r="D56" t="s">
+        <v>85</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C57" s="5"/>
+      <c r="D57" t="s">
+        <v>87</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C58" s="5"/>
+      <c r="D58" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="59" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C59" s="5"/>
+      <c r="D59" t="s">
+        <v>195</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C60" s="5"/>
+      <c r="D60" t="s">
+        <v>89</v>
+      </c>
+      <c r="F60">
+        <v>2</v>
+      </c>
+      <c r="J60" s="6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="61" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C61" s="5"/>
+      <c r="D61" t="s">
+        <v>91</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="J61" s="6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="62" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C62" s="11"/>
+      <c r="D62" t="s">
+        <v>93</v>
+      </c>
+      <c r="J62" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="63" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C63" s="5"/>
+      <c r="D63" t="s">
+        <v>198</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="J63" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="64" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C64" s="5"/>
+      <c r="D64" t="s">
+        <v>200</v>
+      </c>
+      <c r="F64" t="s">
+        <v>159</v>
+      </c>
+      <c r="G64" t="s">
+        <v>159</v>
+      </c>
+      <c r="J64" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="65" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>97</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="J65" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="66" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C66" s="5"/>
+      <c r="D66" t="s">
+        <v>202</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>